<commit_message>
Added AOCM text to ALFS chapter - added more graduate student groups for food security
</commit_message>
<xml_diff>
--- a/data/UCGSES.xlsx
+++ b/data/UCGSES.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanolan\OneDrive\IR_Folder\UCSD_Gaps_Quarto\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A439661B-23F8-40D3-A10B-A9D93CABA0D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EFA0F63-897B-4CF6-BAE9-3BC0C8F2CB5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{61FCD85B-1D55-4F53-8AAE-887E8D8E82D6}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9844" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9934" uniqueCount="75">
   <si>
     <t>q</t>
   </si>
@@ -262,6 +262,9 @@
   <si>
     <t>the career support I receive in my program</t>
   </si>
+  <si>
+    <t>Graduate Professional</t>
+  </si>
 </sst>
 </file>
 
@@ -317,7 +320,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -336,6 +339,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -645,7 +651,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -653,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1E9CEE1-CF8E-498D-873A-AA06707249A5}">
-  <dimension ref="A1:P1640"/>
+  <dimension ref="A1:P1655"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1563" workbookViewId="0">
-      <selection activeCell="D1639" sqref="D1587:D1639"/>
+    <sheetView tabSelected="1" topLeftCell="A1637" workbookViewId="0">
+      <selection activeCell="I1656" sqref="I1656"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -53001,6 +53007,486 @@
         <v>6</v>
       </c>
     </row>
+    <row r="1641" spans="1:10">
+      <c r="A1641" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1641" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1641" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1641" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1641">
+        <v>2021</v>
+      </c>
+      <c r="F1641" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1641" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1641">
+        <v>3</v>
+      </c>
+      <c r="I1641">
+        <v>0.72</v>
+      </c>
+      <c r="J1641">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="1642" spans="1:10">
+      <c r="A1642" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1642" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1642" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1642" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1642">
+        <v>2021</v>
+      </c>
+      <c r="F1642" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1642" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1642">
+        <v>2</v>
+      </c>
+      <c r="I1642">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J1642">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1643" spans="1:10">
+      <c r="A1643" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1643" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1643" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1643" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1643">
+        <v>2021</v>
+      </c>
+      <c r="F1643" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1643" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1643">
+        <v>1</v>
+      </c>
+      <c r="I1643">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J1643">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1644" spans="1:10">
+      <c r="A1644" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1644" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1644" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1644" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1644">
+        <v>2021</v>
+      </c>
+      <c r="F1644" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1644" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1644">
+        <v>3</v>
+      </c>
+      <c r="I1644">
+        <v>0.81</v>
+      </c>
+      <c r="J1644">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="1645" spans="1:10">
+      <c r="A1645" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1645" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1645" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1645" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1645">
+        <v>2021</v>
+      </c>
+      <c r="F1645" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1645" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1645">
+        <v>2</v>
+      </c>
+      <c r="I1645">
+        <v>0.11</v>
+      </c>
+      <c r="J1645">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="1646" spans="1:10">
+      <c r="A1646" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1646" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1646" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1646" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1646">
+        <v>2021</v>
+      </c>
+      <c r="F1646" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1646" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1646">
+        <v>1</v>
+      </c>
+      <c r="I1646">
+        <v>0.08</v>
+      </c>
+      <c r="J1646">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="1647" spans="1:10">
+      <c r="A1647" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1647" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1647" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1647" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1647">
+        <v>2021</v>
+      </c>
+      <c r="F1647" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1647" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1647">
+        <v>3</v>
+      </c>
+      <c r="I1647">
+        <v>0.77</v>
+      </c>
+      <c r="J1647">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="1648" spans="1:10">
+      <c r="A1648" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1648" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1648" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1648" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1648">
+        <v>2021</v>
+      </c>
+      <c r="F1648" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1648" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1648">
+        <v>2</v>
+      </c>
+      <c r="I1648">
+        <v>0.12</v>
+      </c>
+      <c r="J1648">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="1649" spans="1:10">
+      <c r="A1649" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1649" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1649" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1649" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1649">
+        <v>2021</v>
+      </c>
+      <c r="F1649" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1649" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1649">
+        <v>1</v>
+      </c>
+      <c r="I1649">
+        <v>0.1</v>
+      </c>
+      <c r="J1649">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="1650" spans="1:10">
+      <c r="A1650" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1650" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1650" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1650" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1650">
+        <v>2021</v>
+      </c>
+      <c r="F1650" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1650" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1650">
+        <v>3</v>
+      </c>
+      <c r="I1650">
+        <v>0.81</v>
+      </c>
+      <c r="J1650">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="1651" spans="1:10">
+      <c r="A1651" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1651" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1651" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1651" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1651">
+        <v>2021</v>
+      </c>
+      <c r="F1651" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1651" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1651">
+        <v>2</v>
+      </c>
+      <c r="I1651">
+        <v>0.11</v>
+      </c>
+      <c r="J1651">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1652" spans="1:10">
+      <c r="A1652" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1652" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1652" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1652" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1652">
+        <v>2021</v>
+      </c>
+      <c r="F1652" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1652" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1652">
+        <v>1</v>
+      </c>
+      <c r="I1652">
+        <v>0.08</v>
+      </c>
+      <c r="J1652">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1653" spans="1:10">
+      <c r="A1653" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1653" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1653" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1653" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1653">
+        <v>2021</v>
+      </c>
+      <c r="F1653" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1653" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1653">
+        <v>3</v>
+      </c>
+      <c r="I1653">
+        <v>0.81</v>
+      </c>
+      <c r="J1653">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="1654" spans="1:10">
+      <c r="A1654" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1654" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1654" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1654" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1654">
+        <v>2021</v>
+      </c>
+      <c r="F1654" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1654" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1654">
+        <v>2</v>
+      </c>
+      <c r="I1654">
+        <v>0.1</v>
+      </c>
+      <c r="J1654">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1655" spans="1:10">
+      <c r="A1655" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1655" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1655" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1655" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1655">
+        <v>2021</v>
+      </c>
+      <c r="F1655" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1655" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1655">
+        <v>1</v>
+      </c>
+      <c r="I1655">
+        <v>0.09</v>
+      </c>
+      <c r="J1655">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J1640" xr:uid="{D1E9CEE1-CF8E-498D-873A-AA06707249A5}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J626">

</xml_diff>

<commit_message>
Cleaned up a few more errors in MCA, and added UCUES advising questions from 2020
</commit_message>
<xml_diff>
--- a/data/UCGSES.xlsx
+++ b/data/UCGSES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanolan\OneDrive\IR_Folder\UCSD_Gaps_Quarto\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EFA0F63-897B-4CF6-BAE9-3BC0C8F2CB5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC584369-D176-4FAA-979D-80D977EAB675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{61FCD85B-1D55-4F53-8AAE-887E8D8E82D6}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9934" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10708" uniqueCount="76">
   <si>
     <t>q</t>
   </si>
@@ -265,6 +265,9 @@
   <si>
     <t>Graduate Professional</t>
   </si>
+  <si>
+    <t>Professional Practice</t>
+  </si>
 </sst>
 </file>
 
@@ -320,7 +323,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -339,9 +342,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -659,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1E9CEE1-CF8E-498D-873A-AA06707249A5}">
-  <dimension ref="A1:P1655"/>
+  <dimension ref="A1:P1784"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1637" workbookViewId="0">
-      <selection activeCell="I1656" sqref="I1656"/>
+    <sheetView tabSelected="1" topLeftCell="A1766" workbookViewId="0">
+      <selection activeCell="D1785" sqref="D1785"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -53206,7 +53206,7 @@
       <c r="B1647" t="s">
         <v>33</v>
       </c>
-      <c r="C1647" s="8" t="s">
+      <c r="C1647" s="4" t="s">
         <v>49</v>
       </c>
       <c r="D1647" t="s">
@@ -53238,7 +53238,7 @@
       <c r="B1648" t="s">
         <v>33</v>
       </c>
-      <c r="C1648" s="8" t="s">
+      <c r="C1648" s="4" t="s">
         <v>49</v>
       </c>
       <c r="D1648" t="s">
@@ -53263,14 +53263,14 @@
         <v>69</v>
       </c>
     </row>
-    <row r="1649" spans="1:10">
+    <row r="1649" spans="1:13">
       <c r="A1649" t="s">
         <v>34</v>
       </c>
       <c r="B1649" t="s">
         <v>33</v>
       </c>
-      <c r="C1649" s="8" t="s">
+      <c r="C1649" s="4" t="s">
         <v>49</v>
       </c>
       <c r="D1649" t="s">
@@ -53295,14 +53295,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="1650" spans="1:10">
+    <row r="1650" spans="1:13">
       <c r="A1650" t="s">
         <v>34</v>
       </c>
       <c r="B1650" t="s">
         <v>33</v>
       </c>
-      <c r="C1650" s="8" t="s">
+      <c r="C1650" s="4" t="s">
         <v>50</v>
       </c>
       <c r="D1650" t="s">
@@ -53327,14 +53327,14 @@
         <v>158</v>
       </c>
     </row>
-    <row r="1651" spans="1:10">
+    <row r="1651" spans="1:13">
       <c r="A1651" t="s">
         <v>34</v>
       </c>
       <c r="B1651" t="s">
         <v>33</v>
       </c>
-      <c r="C1651" s="8" t="s">
+      <c r="C1651" s="4" t="s">
         <v>50</v>
       </c>
       <c r="D1651" t="s">
@@ -53359,14 +53359,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="1652" spans="1:10">
+    <row r="1652" spans="1:13">
       <c r="A1652" t="s">
         <v>34</v>
       </c>
       <c r="B1652" t="s">
         <v>33</v>
       </c>
-      <c r="C1652" s="8" t="s">
+      <c r="C1652" s="4" t="s">
         <v>50</v>
       </c>
       <c r="D1652" t="s">
@@ -53391,14 +53391,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="1653" spans="1:10">
+    <row r="1653" spans="1:13">
       <c r="A1653" t="s">
         <v>34</v>
       </c>
       <c r="B1653" t="s">
         <v>33</v>
       </c>
-      <c r="C1653" s="8" t="s">
+      <c r="C1653" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D1653" t="s">
@@ -53423,14 +53423,14 @@
         <v>111</v>
       </c>
     </row>
-    <row r="1654" spans="1:10">
+    <row r="1654" spans="1:13">
       <c r="A1654" t="s">
         <v>34</v>
       </c>
       <c r="B1654" t="s">
         <v>33</v>
       </c>
-      <c r="C1654" s="8" t="s">
+      <c r="C1654" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D1654" t="s">
@@ -53455,14 +53455,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="1655" spans="1:10">
+    <row r="1655" spans="1:13">
       <c r="A1655" t="s">
         <v>34</v>
       </c>
       <c r="B1655" t="s">
         <v>33</v>
       </c>
-      <c r="C1655" s="8" t="s">
+      <c r="C1655" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D1655" t="s">
@@ -53485,6 +53485,3966 @@
       </c>
       <c r="J1655">
         <v>7</v>
+      </c>
+    </row>
+    <row r="1656" spans="1:13">
+      <c r="A1656" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1656" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1656" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1656" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1656">
+        <v>2021</v>
+      </c>
+      <c r="F1656" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1656" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1656">
+        <v>6</v>
+      </c>
+      <c r="I1656">
+        <v>0.16129032300000001</v>
+      </c>
+      <c r="J1656">
+        <v>5</v>
+      </c>
+      <c r="M1656" s="7"/>
+    </row>
+    <row r="1657" spans="1:13">
+      <c r="A1657" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1657" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1657" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1657" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1657">
+        <v>2021</v>
+      </c>
+      <c r="F1657" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1657" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1657">
+        <v>6</v>
+      </c>
+      <c r="I1657">
+        <v>0.16129032300000001</v>
+      </c>
+      <c r="J1657">
+        <v>5</v>
+      </c>
+      <c r="M1657" s="7"/>
+    </row>
+    <row r="1658" spans="1:13">
+      <c r="A1658" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1658" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1658" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1658" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1658">
+        <v>2021</v>
+      </c>
+      <c r="F1658" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1658" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1658">
+        <v>6</v>
+      </c>
+      <c r="I1658">
+        <v>0.16129032300000001</v>
+      </c>
+      <c r="J1658">
+        <v>5</v>
+      </c>
+      <c r="M1658" s="7"/>
+    </row>
+    <row r="1659" spans="1:13">
+      <c r="A1659" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1659" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1659" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1659" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1659">
+        <v>2021</v>
+      </c>
+      <c r="F1659" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1659" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1659">
+        <v>6</v>
+      </c>
+      <c r="M1659" s="7"/>
+    </row>
+    <row r="1660" spans="1:13">
+      <c r="A1660" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1660" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1660" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1660" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1660">
+        <v>2021</v>
+      </c>
+      <c r="F1660" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1660" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1660">
+        <v>5</v>
+      </c>
+      <c r="I1660">
+        <v>0.19354838699999999</v>
+      </c>
+      <c r="J1660">
+        <v>6</v>
+      </c>
+      <c r="M1660" s="7"/>
+    </row>
+    <row r="1661" spans="1:13">
+      <c r="A1661" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1661" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1661" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1661" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1661">
+        <v>2021</v>
+      </c>
+      <c r="F1661" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1661" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1661">
+        <v>5</v>
+      </c>
+      <c r="I1661">
+        <v>0.22580645199999999</v>
+      </c>
+      <c r="J1661">
+        <v>7</v>
+      </c>
+      <c r="M1661" s="7"/>
+    </row>
+    <row r="1662" spans="1:13">
+      <c r="A1662" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1662" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1662" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1662" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1662">
+        <v>2021</v>
+      </c>
+      <c r="F1662" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1662" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1662">
+        <v>5</v>
+      </c>
+      <c r="I1662">
+        <v>0.16129032300000001</v>
+      </c>
+      <c r="J1662">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1663" spans="1:13">
+      <c r="A1663" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1663" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1663" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1663" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1663">
+        <v>2021</v>
+      </c>
+      <c r="F1663" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1663" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1663">
+        <v>5</v>
+      </c>
+      <c r="I1663">
+        <v>0.19354838699999999</v>
+      </c>
+      <c r="J1663">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1664" spans="1:13">
+      <c r="A1664" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1664" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1664" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1664" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1664">
+        <v>2021</v>
+      </c>
+      <c r="F1664" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1664" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1664">
+        <v>4</v>
+      </c>
+      <c r="I1664">
+        <v>0.29032258100000002</v>
+      </c>
+      <c r="J1664">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1665" spans="1:10">
+      <c r="A1665" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1665" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1665" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1665" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1665">
+        <v>2021</v>
+      </c>
+      <c r="F1665" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1665" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1665">
+        <v>4</v>
+      </c>
+      <c r="I1665">
+        <v>0.29032258100000002</v>
+      </c>
+      <c r="J1665">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1666" spans="1:10">
+      <c r="A1666" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1666" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1666" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1666" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1666">
+        <v>2021</v>
+      </c>
+      <c r="F1666" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1666" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1666">
+        <v>4</v>
+      </c>
+      <c r="I1666">
+        <v>0.35483871</v>
+      </c>
+      <c r="J1666">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1667" spans="1:10">
+      <c r="A1667" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1667" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1667" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1667" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1667">
+        <v>2021</v>
+      </c>
+      <c r="F1667" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1667" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1667">
+        <v>4</v>
+      </c>
+      <c r="I1667">
+        <v>0.19354838699999999</v>
+      </c>
+      <c r="J1667">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1668" spans="1:10">
+      <c r="A1668" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1668" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1668" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1668" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1668">
+        <v>2021</v>
+      </c>
+      <c r="F1668" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1668" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1668">
+        <v>3</v>
+      </c>
+      <c r="I1668">
+        <v>0.16129032300000001</v>
+      </c>
+      <c r="J1668">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1669" spans="1:10">
+      <c r="A1669" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1669" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1669" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1669" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1669">
+        <v>2021</v>
+      </c>
+      <c r="F1669" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1669" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1669">
+        <v>3</v>
+      </c>
+      <c r="I1669">
+        <v>0.16129032300000001</v>
+      </c>
+      <c r="J1669">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1670" spans="1:10">
+      <c r="A1670" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1670" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1670" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1670" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1670">
+        <v>2021</v>
+      </c>
+      <c r="F1670" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1670" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1670">
+        <v>3</v>
+      </c>
+      <c r="I1670">
+        <v>0.12903225800000001</v>
+      </c>
+      <c r="J1670">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1671" spans="1:10">
+      <c r="A1671" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1671" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1671" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1671" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1671">
+        <v>2021</v>
+      </c>
+      <c r="F1671" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1671" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1671">
+        <v>3</v>
+      </c>
+      <c r="I1671">
+        <v>0.22580645199999999</v>
+      </c>
+      <c r="J1671">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1672" spans="1:10">
+      <c r="A1672" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1672" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1672" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1672" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1672">
+        <v>2021</v>
+      </c>
+      <c r="F1672" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1672" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1672">
+        <v>2</v>
+      </c>
+      <c r="I1672">
+        <v>0.12903225800000001</v>
+      </c>
+      <c r="J1672">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1673" spans="1:10">
+      <c r="A1673" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1673" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1673" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1673" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1673">
+        <v>2021</v>
+      </c>
+      <c r="F1673" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1673" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1673">
+        <v>2</v>
+      </c>
+      <c r="I1673">
+        <v>0.16129032300000001</v>
+      </c>
+      <c r="J1673">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1674" spans="1:10">
+      <c r="A1674" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1674" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1674" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1674" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1674">
+        <v>2021</v>
+      </c>
+      <c r="F1674" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1674" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1674">
+        <v>2</v>
+      </c>
+      <c r="I1674">
+        <v>0.16129032300000001</v>
+      </c>
+      <c r="J1674">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1675" spans="1:10">
+      <c r="A1675" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1675" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1675" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1675" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1675">
+        <v>2021</v>
+      </c>
+      <c r="F1675" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1675" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1675">
+        <v>2</v>
+      </c>
+      <c r="I1675">
+        <v>0.19354838699999999</v>
+      </c>
+      <c r="J1675">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1676" spans="1:10">
+      <c r="A1676" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1676" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1676" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1676" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1676">
+        <v>2021</v>
+      </c>
+      <c r="F1676" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1676" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1676">
+        <v>1</v>
+      </c>
+      <c r="I1676">
+        <v>6.4516129000000005E-2</v>
+      </c>
+      <c r="J1676">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1677" spans="1:10">
+      <c r="A1677" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1677" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1677" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1677" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1677">
+        <v>2021</v>
+      </c>
+      <c r="F1677" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1677" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1677">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1678" spans="1:10">
+      <c r="A1678" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1678" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1678" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1678" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1678">
+        <v>2021</v>
+      </c>
+      <c r="F1678" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1678" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1678">
+        <v>1</v>
+      </c>
+      <c r="I1678">
+        <v>3.2258065000000002E-2</v>
+      </c>
+      <c r="J1678">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1679" spans="1:10">
+      <c r="A1679" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1679" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1679" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1679" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1679">
+        <v>2021</v>
+      </c>
+      <c r="F1679" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1679" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1679">
+        <v>1</v>
+      </c>
+      <c r="I1679">
+        <v>0.19354838699999999</v>
+      </c>
+      <c r="J1679">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1680" spans="1:10">
+      <c r="A1680" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1680" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1680" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1680" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1680">
+        <v>2021</v>
+      </c>
+      <c r="F1680" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1680" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1680">
+        <v>6</v>
+      </c>
+      <c r="I1680">
+        <v>0.4</v>
+      </c>
+      <c r="J1680">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1681" spans="1:10">
+      <c r="A1681" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1681" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1681" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1681" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1681">
+        <v>2021</v>
+      </c>
+      <c r="F1681" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1681" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1681">
+        <v>6</v>
+      </c>
+      <c r="I1681">
+        <v>0.46875</v>
+      </c>
+      <c r="J1681">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1682" spans="1:10">
+      <c r="A1682" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1682" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1682" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1682" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1682">
+        <v>2021</v>
+      </c>
+      <c r="F1682" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1682" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1682">
+        <v>6</v>
+      </c>
+      <c r="I1682">
+        <v>0.52777777800000003</v>
+      </c>
+      <c r="J1682">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1683" spans="1:10">
+      <c r="A1683" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1683" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1683" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1683" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1683">
+        <v>2021</v>
+      </c>
+      <c r="F1683" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1683" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1683">
+        <v>6</v>
+      </c>
+      <c r="I1683">
+        <v>0.484848485</v>
+      </c>
+      <c r="J1683">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1684" spans="1:10">
+      <c r="A1684" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1684" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1684" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1684" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1684">
+        <v>2021</v>
+      </c>
+      <c r="F1684" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1684" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1684">
+        <v>6</v>
+      </c>
+      <c r="I1684">
+        <v>0.52941176499999998</v>
+      </c>
+      <c r="J1684">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1685" spans="1:10">
+      <c r="A1685" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1685" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1685" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1685" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1685">
+        <v>2021</v>
+      </c>
+      <c r="F1685" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1685" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1685">
+        <v>6</v>
+      </c>
+      <c r="I1685">
+        <v>0.485714286</v>
+      </c>
+      <c r="J1685">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1686" spans="1:10">
+      <c r="A1686" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1686" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1686" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1686" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1686">
+        <v>2021</v>
+      </c>
+      <c r="F1686" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1686" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1686">
+        <v>6</v>
+      </c>
+      <c r="I1686">
+        <v>0.45714285700000001</v>
+      </c>
+      <c r="J1686">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1687" spans="1:10">
+      <c r="A1687" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1687" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1687" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1687" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1687">
+        <v>2021</v>
+      </c>
+      <c r="F1687" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1687" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1687">
+        <v>6</v>
+      </c>
+      <c r="I1687">
+        <v>0.321428571</v>
+      </c>
+      <c r="J1687">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1688" spans="1:10">
+      <c r="A1688" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1688" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1688" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1688" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1688">
+        <v>2021</v>
+      </c>
+      <c r="F1688" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1688" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1688">
+        <v>6</v>
+      </c>
+      <c r="I1688">
+        <v>0.57575757599999999</v>
+      </c>
+      <c r="J1688">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1689" spans="1:10">
+      <c r="A1689" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1689" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1689" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1689" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1689">
+        <v>2021</v>
+      </c>
+      <c r="F1689" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1689" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1689">
+        <v>6</v>
+      </c>
+      <c r="I1689">
+        <v>0.38888888900000002</v>
+      </c>
+      <c r="J1689">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1690" spans="1:10">
+      <c r="A1690" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1690" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1690" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1690" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1690">
+        <v>2021</v>
+      </c>
+      <c r="F1690" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1690" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1690">
+        <v>5</v>
+      </c>
+      <c r="I1690">
+        <v>0.2</v>
+      </c>
+      <c r="J1690">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1691" spans="1:10">
+      <c r="A1691" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1691" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1691" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1691" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1691">
+        <v>2021</v>
+      </c>
+      <c r="F1691" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1691" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1691">
+        <v>5</v>
+      </c>
+      <c r="I1691">
+        <v>0.1875</v>
+      </c>
+      <c r="J1691">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1692" spans="1:10">
+      <c r="A1692" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1692" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1692" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1692" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1692">
+        <v>2021</v>
+      </c>
+      <c r="F1692" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1692" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1692">
+        <v>5</v>
+      </c>
+      <c r="I1692">
+        <v>0.222222222</v>
+      </c>
+      <c r="J1692">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1693" spans="1:10">
+      <c r="A1693" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1693" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1693" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1693" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1693">
+        <v>2021</v>
+      </c>
+      <c r="F1693" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1693" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1693">
+        <v>5</v>
+      </c>
+      <c r="I1693">
+        <v>0.12121212100000001</v>
+      </c>
+      <c r="J1693">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1694" spans="1:10">
+      <c r="A1694" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1694" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1694" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1694" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1694">
+        <v>2021</v>
+      </c>
+      <c r="F1694" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1694" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1694">
+        <v>5</v>
+      </c>
+      <c r="I1694">
+        <v>0.20588235299999999</v>
+      </c>
+      <c r="J1694">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1695" spans="1:10">
+      <c r="A1695" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1695" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1695" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1695" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1695">
+        <v>2021</v>
+      </c>
+      <c r="F1695" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1695" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1695">
+        <v>5</v>
+      </c>
+      <c r="I1695">
+        <v>0.171428571</v>
+      </c>
+      <c r="J1695">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1696" spans="1:10">
+      <c r="A1696" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1696" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1696" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1696" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1696">
+        <v>2021</v>
+      </c>
+      <c r="F1696" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1696" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1696">
+        <v>5</v>
+      </c>
+      <c r="I1696">
+        <v>8.5714286000000001E-2</v>
+      </c>
+      <c r="J1696">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1697" spans="1:10">
+      <c r="A1697" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1697" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1697" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1697" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1697">
+        <v>2021</v>
+      </c>
+      <c r="F1697" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1697" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1697">
+        <v>5</v>
+      </c>
+      <c r="I1697">
+        <v>7.1428570999999996E-2</v>
+      </c>
+      <c r="J1697">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1698" spans="1:10">
+      <c r="A1698" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1698" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1698" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1698" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1698">
+        <v>2021</v>
+      </c>
+      <c r="F1698" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1698" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1698">
+        <v>5</v>
+      </c>
+      <c r="I1698">
+        <v>0.212121212</v>
+      </c>
+      <c r="J1698">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1699" spans="1:10">
+      <c r="A1699" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1699" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1699" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1699" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1699">
+        <v>2021</v>
+      </c>
+      <c r="F1699" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1699" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1699">
+        <v>5</v>
+      </c>
+      <c r="I1699">
+        <v>0.13888888899999999</v>
+      </c>
+      <c r="J1699">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1700" spans="1:10">
+      <c r="A1700" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1700" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1700" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1700" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1700">
+        <v>2021</v>
+      </c>
+      <c r="F1700" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1700" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1700">
+        <v>4</v>
+      </c>
+      <c r="I1700">
+        <v>0.34285714299999998</v>
+      </c>
+      <c r="J1700">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1701" spans="1:10">
+      <c r="A1701" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1701" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1701" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1701" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1701">
+        <v>2021</v>
+      </c>
+      <c r="F1701" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1701" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1701">
+        <v>4</v>
+      </c>
+      <c r="I1701">
+        <v>0.28125</v>
+      </c>
+      <c r="J1701">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1702" spans="1:10">
+      <c r="A1702" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1702" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1702" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1702" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1702">
+        <v>2021</v>
+      </c>
+      <c r="F1702" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1702" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1702">
+        <v>4</v>
+      </c>
+      <c r="I1702">
+        <v>0.19444444399999999</v>
+      </c>
+      <c r="J1702">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1703" spans="1:10">
+      <c r="A1703" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1703" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1703" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1703" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1703">
+        <v>2021</v>
+      </c>
+      <c r="F1703" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1703" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1703">
+        <v>4</v>
+      </c>
+      <c r="I1703">
+        <v>0.27272727299999999</v>
+      </c>
+      <c r="J1703">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1704" spans="1:10">
+      <c r="A1704" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1704" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1704" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1704" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1704">
+        <v>2021</v>
+      </c>
+      <c r="F1704" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1704" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1704">
+        <v>4</v>
+      </c>
+      <c r="I1704">
+        <v>0.147058824</v>
+      </c>
+      <c r="J1704">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1705" spans="1:10">
+      <c r="A1705" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1705" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1705" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1705" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1705">
+        <v>2021</v>
+      </c>
+      <c r="F1705" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1705" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1705">
+        <v>4</v>
+      </c>
+      <c r="I1705">
+        <v>0.2</v>
+      </c>
+      <c r="J1705">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1706" spans="1:10">
+      <c r="A1706" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1706" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1706" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1706" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1706">
+        <v>2021</v>
+      </c>
+      <c r="F1706" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1706" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1706">
+        <v>4</v>
+      </c>
+      <c r="I1706">
+        <v>0.257142857</v>
+      </c>
+      <c r="J1706">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1707" spans="1:10">
+      <c r="A1707" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1707" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1707" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1707" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1707">
+        <v>2021</v>
+      </c>
+      <c r="F1707" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1707" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1707">
+        <v>4</v>
+      </c>
+      <c r="I1707">
+        <v>0.428571429</v>
+      </c>
+      <c r="J1707">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1708" spans="1:10">
+      <c r="A1708" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1708" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1708" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1708" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1708">
+        <v>2021</v>
+      </c>
+      <c r="F1708" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1708" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1708">
+        <v>4</v>
+      </c>
+      <c r="I1708">
+        <v>0.18181818199999999</v>
+      </c>
+      <c r="J1708">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1709" spans="1:10">
+      <c r="A1709" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1709" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1709" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1709" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1709">
+        <v>2021</v>
+      </c>
+      <c r="F1709" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1709" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1709">
+        <v>4</v>
+      </c>
+      <c r="I1709">
+        <v>0.36111111099999998</v>
+      </c>
+      <c r="J1709">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1710" spans="1:10">
+      <c r="A1710" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1710" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1710" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1710" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1710">
+        <v>2021</v>
+      </c>
+      <c r="F1710" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1710" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1710">
+        <v>3</v>
+      </c>
+      <c r="I1710">
+        <v>5.7142856999999998E-2</v>
+      </c>
+      <c r="J1710">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1711" spans="1:10">
+      <c r="A1711" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1711" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1711" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1711" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1711">
+        <v>2021</v>
+      </c>
+      <c r="F1711" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1711" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1711">
+        <v>3</v>
+      </c>
+      <c r="I1711">
+        <v>6.25E-2</v>
+      </c>
+      <c r="J1711">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1712" spans="1:10">
+      <c r="A1712" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1712" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1712" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1712" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1712">
+        <v>2021</v>
+      </c>
+      <c r="F1712" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1712" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1712">
+        <v>3</v>
+      </c>
+      <c r="I1712">
+        <v>5.5555555999999999E-2</v>
+      </c>
+      <c r="J1712">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1713" spans="1:10">
+      <c r="A1713" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1713" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1713" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1713" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1713">
+        <v>2021</v>
+      </c>
+      <c r="F1713" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1713" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1713">
+        <v>3</v>
+      </c>
+      <c r="I1713">
+        <v>9.0909090999999997E-2</v>
+      </c>
+      <c r="J1713">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1714" spans="1:10">
+      <c r="A1714" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1714" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1714" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1714" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1714">
+        <v>2021</v>
+      </c>
+      <c r="F1714" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1714" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1714">
+        <v>3</v>
+      </c>
+      <c r="I1714">
+        <v>8.8235294000000006E-2</v>
+      </c>
+      <c r="J1714">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1715" spans="1:10">
+      <c r="A1715" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1715" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1715" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1715" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1715">
+        <v>2021</v>
+      </c>
+      <c r="F1715" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1715" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1715">
+        <v>3</v>
+      </c>
+      <c r="I1715">
+        <v>0.14285714299999999</v>
+      </c>
+      <c r="J1715">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1716" spans="1:10">
+      <c r="A1716" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1716" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1716" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1716" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1716">
+        <v>2021</v>
+      </c>
+      <c r="F1716" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1716" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1716">
+        <v>3</v>
+      </c>
+      <c r="I1716">
+        <v>0.171428571</v>
+      </c>
+      <c r="J1716">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1717" spans="1:10">
+      <c r="A1717" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1717" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1717" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1717" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1717">
+        <v>2021</v>
+      </c>
+      <c r="F1717" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1717" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1717">
+        <v>3</v>
+      </c>
+      <c r="I1717">
+        <v>0.10714285699999999</v>
+      </c>
+      <c r="J1717">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1718" spans="1:10">
+      <c r="A1718" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1718" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1718" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1718" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1718">
+        <v>2021</v>
+      </c>
+      <c r="F1718" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1718" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1718">
+        <v>3</v>
+      </c>
+      <c r="I1718">
+        <v>3.0303030000000002E-2</v>
+      </c>
+      <c r="J1718">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1719" spans="1:10">
+      <c r="A1719" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1719" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1719" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1719" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1719">
+        <v>2021</v>
+      </c>
+      <c r="F1719" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1719" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1719">
+        <v>3</v>
+      </c>
+      <c r="I1719">
+        <v>8.3333332999999996E-2</v>
+      </c>
+      <c r="J1719">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1720" spans="1:10">
+      <c r="A1720" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1720" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1720" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1720" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1720">
+        <v>2021</v>
+      </c>
+      <c r="F1720" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1720" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1720">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1721" spans="1:10">
+      <c r="A1721" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1721" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1721" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1721" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1721">
+        <v>2021</v>
+      </c>
+      <c r="F1721" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1721" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1721">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1722" spans="1:10">
+      <c r="A1722" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1722" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1722" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1722" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1722">
+        <v>2021</v>
+      </c>
+      <c r="F1722" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1722" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1722">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1723" spans="1:10">
+      <c r="A1723" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1723" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1723" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1723" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1723">
+        <v>2021</v>
+      </c>
+      <c r="F1723" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1723" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1723">
+        <v>2</v>
+      </c>
+      <c r="I1723">
+        <v>3.0303030000000002E-2</v>
+      </c>
+      <c r="J1723">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1724" spans="1:10">
+      <c r="A1724" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1724" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1724" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1724" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1724">
+        <v>2021</v>
+      </c>
+      <c r="F1724" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1724" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1724">
+        <v>2</v>
+      </c>
+      <c r="I1724">
+        <v>2.9411764999999999E-2</v>
+      </c>
+      <c r="J1724">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1725" spans="1:10">
+      <c r="A1725" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1725" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1725" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1725" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1725">
+        <v>2021</v>
+      </c>
+      <c r="F1725" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1725" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1725">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1726" spans="1:10">
+      <c r="A1726" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1726" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1726" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1726" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1726">
+        <v>2021</v>
+      </c>
+      <c r="F1726" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1726" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1726">
+        <v>2</v>
+      </c>
+      <c r="I1726">
+        <v>2.8571428999999999E-2</v>
+      </c>
+      <c r="J1726">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1727" spans="1:10">
+      <c r="A1727" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1727" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1727" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1727" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1727">
+        <v>2021</v>
+      </c>
+      <c r="F1727" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1727" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1727">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1728" spans="1:10">
+      <c r="A1728" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1728" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1728" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1728" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1728">
+        <v>2021</v>
+      </c>
+      <c r="F1728" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1728" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1728">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1729" spans="1:10">
+      <c r="A1729" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1729" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1729" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1729" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1729">
+        <v>2021</v>
+      </c>
+      <c r="F1729" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1729" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1729">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1730" spans="1:10">
+      <c r="A1730" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1730" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1730" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1730" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1730">
+        <v>2021</v>
+      </c>
+      <c r="F1730" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1730" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1730">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1731" spans="1:10">
+      <c r="A1731" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1731" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1731" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1731" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1731">
+        <v>2021</v>
+      </c>
+      <c r="F1731" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1731" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1731">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1732" spans="1:10">
+      <c r="A1732" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1732" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1732" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1732" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1732">
+        <v>2021</v>
+      </c>
+      <c r="F1732" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1732" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1732">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1733" spans="1:10">
+      <c r="A1733" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1733" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1733" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1733" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1733">
+        <v>2021</v>
+      </c>
+      <c r="F1733" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1733" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1733">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1734" spans="1:10">
+      <c r="A1734" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1734" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1734" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1734" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1734">
+        <v>2021</v>
+      </c>
+      <c r="F1734" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1734" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1734">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1735" spans="1:10">
+      <c r="A1735" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1735" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1735" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1735" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1735">
+        <v>2021</v>
+      </c>
+      <c r="F1735" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1735" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1735">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1736" spans="1:10">
+      <c r="A1736" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1736" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1736" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1736" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1736">
+        <v>2021</v>
+      </c>
+      <c r="F1736" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1736" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1736">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1737" spans="1:10">
+      <c r="A1737" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1737" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1737" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1737" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1737">
+        <v>2021</v>
+      </c>
+      <c r="F1737" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1737" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1737">
+        <v>1</v>
+      </c>
+      <c r="I1737">
+        <v>7.1428570999999996E-2</v>
+      </c>
+      <c r="J1737">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1738" spans="1:10">
+      <c r="A1738" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1738" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1738" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1738" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1738">
+        <v>2021</v>
+      </c>
+      <c r="F1738" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1738" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1738">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1739" spans="1:10">
+      <c r="A1739" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1739" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1739" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1739" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1739">
+        <v>2021</v>
+      </c>
+      <c r="F1739" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1739" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1739">
+        <v>1</v>
+      </c>
+      <c r="I1739">
+        <v>2.7777777999999999E-2</v>
+      </c>
+      <c r="J1739">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1740" spans="1:10">
+      <c r="A1740" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1740" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1740" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1740" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1740">
+        <v>2021</v>
+      </c>
+      <c r="F1740" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1740" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1740">
+        <v>6</v>
+      </c>
+      <c r="I1740">
+        <v>0.38709677399999998</v>
+      </c>
+      <c r="J1740">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1741" spans="1:10">
+      <c r="A1741" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1741" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1741" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1741" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1741">
+        <v>2021</v>
+      </c>
+      <c r="F1741" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1741" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1741">
+        <v>6</v>
+      </c>
+      <c r="I1741">
+        <v>0.41935483899999998</v>
+      </c>
+      <c r="J1741">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1742" spans="1:10">
+      <c r="A1742" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1742" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1742" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1742" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1742">
+        <v>2021</v>
+      </c>
+      <c r="F1742" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1742" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1742">
+        <v>6</v>
+      </c>
+      <c r="I1742">
+        <v>0.38709677399999998</v>
+      </c>
+      <c r="J1742">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1743" spans="1:10">
+      <c r="A1743" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1743" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1743" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1743" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1743">
+        <v>2021</v>
+      </c>
+      <c r="F1743" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1743" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1743">
+        <v>6</v>
+      </c>
+      <c r="I1743">
+        <v>0.29032258100000002</v>
+      </c>
+      <c r="J1743">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1744" spans="1:10">
+      <c r="A1744" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1744" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1744" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1744" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1744">
+        <v>2021</v>
+      </c>
+      <c r="F1744" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1744" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1744">
+        <v>6</v>
+      </c>
+      <c r="I1744">
+        <v>0.322580645</v>
+      </c>
+      <c r="J1744">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1745" spans="1:10">
+      <c r="A1745" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1745" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1745" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1745" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1745">
+        <v>2021</v>
+      </c>
+      <c r="F1745" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1745" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1745">
+        <v>6</v>
+      </c>
+      <c r="I1745">
+        <v>0.35483871</v>
+      </c>
+      <c r="J1745">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1746" spans="1:10">
+      <c r="A1746" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1746" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1746" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1746" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1746">
+        <v>2021</v>
+      </c>
+      <c r="F1746" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1746" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1746">
+        <v>5</v>
+      </c>
+      <c r="I1746">
+        <v>0.41935483899999998</v>
+      </c>
+      <c r="J1746">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1747" spans="1:10">
+      <c r="A1747" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1747" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1747" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1747" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1747">
+        <v>2021</v>
+      </c>
+      <c r="F1747" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1747" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1747">
+        <v>5</v>
+      </c>
+      <c r="I1747">
+        <v>0.38709677399999998</v>
+      </c>
+      <c r="J1747">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1748" spans="1:10">
+      <c r="A1748" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1748" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1748" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1748" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1748">
+        <v>2021</v>
+      </c>
+      <c r="F1748" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1748" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1748">
+        <v>5</v>
+      </c>
+      <c r="I1748">
+        <v>0.41935483899999998</v>
+      </c>
+      <c r="J1748">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1749" spans="1:10">
+      <c r="A1749" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1749" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1749" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1749" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1749">
+        <v>2021</v>
+      </c>
+      <c r="F1749" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1749" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1749">
+        <v>5</v>
+      </c>
+      <c r="I1749">
+        <v>0.45161290300000001</v>
+      </c>
+      <c r="J1749">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1750" spans="1:10">
+      <c r="A1750" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1750" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1750" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1750" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1750">
+        <v>2021</v>
+      </c>
+      <c r="F1750" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1750" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1750">
+        <v>5</v>
+      </c>
+      <c r="I1750">
+        <v>0.41935483899999998</v>
+      </c>
+      <c r="J1750">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1751" spans="1:10">
+      <c r="A1751" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1751" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1751" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1751" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1751">
+        <v>2021</v>
+      </c>
+      <c r="F1751" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1751" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1751">
+        <v>5</v>
+      </c>
+      <c r="I1751">
+        <v>0.38709677399999998</v>
+      </c>
+      <c r="J1751">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1752" spans="1:10">
+      <c r="A1752" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1752" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1752" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1752" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1752">
+        <v>2021</v>
+      </c>
+      <c r="F1752" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1752" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1752">
+        <v>4</v>
+      </c>
+      <c r="I1752">
+        <v>0.19354838699999999</v>
+      </c>
+      <c r="J1752">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1753" spans="1:10">
+      <c r="A1753" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1753" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1753" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1753" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1753">
+        <v>2021</v>
+      </c>
+      <c r="F1753" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1753" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1753">
+        <v>4</v>
+      </c>
+      <c r="I1753">
+        <v>0.19354838699999999</v>
+      </c>
+      <c r="J1753">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1754" spans="1:10">
+      <c r="A1754" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1754" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1754" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1754" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1754">
+        <v>2021</v>
+      </c>
+      <c r="F1754" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1754" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1754">
+        <v>4</v>
+      </c>
+      <c r="I1754">
+        <v>0.19354838699999999</v>
+      </c>
+      <c r="J1754">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1755" spans="1:10">
+      <c r="A1755" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1755" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1755" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1755" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1755">
+        <v>2021</v>
+      </c>
+      <c r="F1755" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1755" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1755">
+        <v>4</v>
+      </c>
+      <c r="I1755">
+        <v>0.25806451600000002</v>
+      </c>
+      <c r="J1755">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1756" spans="1:10">
+      <c r="A1756" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1756" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1756" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1756" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1756">
+        <v>2021</v>
+      </c>
+      <c r="F1756" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1756" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1756">
+        <v>4</v>
+      </c>
+      <c r="I1756">
+        <v>0.19354838699999999</v>
+      </c>
+      <c r="J1756">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1757" spans="1:10">
+      <c r="A1757" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1757" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1757" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1757" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1757">
+        <v>2021</v>
+      </c>
+      <c r="F1757" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1757" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1757">
+        <v>4</v>
+      </c>
+      <c r="I1757">
+        <v>0.25806451600000002</v>
+      </c>
+      <c r="J1757">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1758" spans="1:10">
+      <c r="A1758" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1758" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1758" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1758" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1758">
+        <v>2021</v>
+      </c>
+      <c r="F1758" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1758" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1758">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1759" spans="1:10">
+      <c r="A1759" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1759" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1759" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1759" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1759">
+        <v>2021</v>
+      </c>
+      <c r="F1759" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1759" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1759">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1760" spans="1:10">
+      <c r="A1760" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1760" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1760" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1760" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1760">
+        <v>2021</v>
+      </c>
+      <c r="F1760" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1760" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1760">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1761" spans="1:10">
+      <c r="A1761" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1761" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1761" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1761" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1761">
+        <v>2021</v>
+      </c>
+      <c r="F1761" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1761" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1761">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1762" spans="1:10">
+      <c r="A1762" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1762" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1762" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1762" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1762">
+        <v>2021</v>
+      </c>
+      <c r="F1762" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1762" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1762">
+        <v>3</v>
+      </c>
+      <c r="I1762">
+        <v>3.2258065000000002E-2</v>
+      </c>
+      <c r="J1762">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1763" spans="1:10">
+      <c r="A1763" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1763" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1763" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1763" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1763">
+        <v>2021</v>
+      </c>
+      <c r="F1763" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1763" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1763">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1764" spans="1:10">
+      <c r="A1764" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1764" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1764" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1764" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1764">
+        <v>2021</v>
+      </c>
+      <c r="F1764" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1764" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1764">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1765" spans="1:10">
+      <c r="A1765" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1765" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1765" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1765" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1765">
+        <v>2021</v>
+      </c>
+      <c r="F1765" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1765" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1765">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1766" spans="1:10">
+      <c r="A1766" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1766" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1766" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1766" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1766">
+        <v>2021</v>
+      </c>
+      <c r="F1766" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1766" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1766">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1767" spans="1:10">
+      <c r="A1767" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1767" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1767" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1767" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1767">
+        <v>2021</v>
+      </c>
+      <c r="F1767" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1767" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1767">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1768" spans="1:10">
+      <c r="A1768" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1768" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1768" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1768" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1768">
+        <v>2021</v>
+      </c>
+      <c r="F1768" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1768" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1768">
+        <v>2</v>
+      </c>
+      <c r="I1768">
+        <v>3.2258065000000002E-2</v>
+      </c>
+      <c r="J1768">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1769" spans="1:10">
+      <c r="A1769" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1769" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1769" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1769" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1769">
+        <v>2021</v>
+      </c>
+      <c r="F1769" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1769" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1769">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1770" spans="1:10">
+      <c r="A1770" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1770" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1770" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1770" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1770">
+        <v>2021</v>
+      </c>
+      <c r="F1770" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1770" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1770">
+        <v>1</v>
+      </c>
+      <c r="I1770">
+        <v>3.2258065000000002E-2</v>
+      </c>
+      <c r="J1770">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1771" spans="1:10">
+      <c r="A1771" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1771" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1771" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1771" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1771">
+        <v>2021</v>
+      </c>
+      <c r="F1771" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1771" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1771">
+        <v>6</v>
+      </c>
+      <c r="I1771">
+        <v>0.41666666699999999</v>
+      </c>
+      <c r="J1771">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1772" spans="1:10">
+      <c r="A1772" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1772" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1772" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1772" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1772">
+        <v>2021</v>
+      </c>
+      <c r="F1772" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1772" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1772">
+        <v>6</v>
+      </c>
+      <c r="I1772">
+        <v>0.36363636399999999</v>
+      </c>
+      <c r="J1772">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1773" spans="1:10">
+      <c r="A1773" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1773" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1773" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1773" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1773">
+        <v>2021</v>
+      </c>
+      <c r="F1773" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1773" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1773">
+        <v>6</v>
+      </c>
+      <c r="I1773">
+        <v>0.36363636399999999</v>
+      </c>
+      <c r="J1773">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1774" spans="1:10">
+      <c r="A1774" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1774" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1774" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1774" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1774">
+        <v>2021</v>
+      </c>
+      <c r="F1774" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1774" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1774">
+        <v>5</v>
+      </c>
+      <c r="I1774">
+        <v>0.33333333300000001</v>
+      </c>
+      <c r="J1774">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1775" spans="1:10">
+      <c r="A1775" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1775" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1775" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1775" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1775">
+        <v>2021</v>
+      </c>
+      <c r="F1775" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1775" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1775">
+        <v>5</v>
+      </c>
+      <c r="I1775">
+        <v>0.303030303</v>
+      </c>
+      <c r="J1775">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1776" spans="1:10">
+      <c r="A1776" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1776" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1776" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1776" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1776">
+        <v>2021</v>
+      </c>
+      <c r="F1776" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1776" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1776">
+        <v>5</v>
+      </c>
+      <c r="I1776">
+        <v>0.36363636399999999</v>
+      </c>
+      <c r="J1776">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1777" spans="1:10">
+      <c r="A1777" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1777" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1777" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1777" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1777">
+        <v>2021</v>
+      </c>
+      <c r="F1777" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1777" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1777">
+        <v>4</v>
+      </c>
+      <c r="I1777">
+        <v>0.25</v>
+      </c>
+      <c r="J1777">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1778" spans="1:10">
+      <c r="A1778" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1778" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1778" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1778" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1778">
+        <v>2021</v>
+      </c>
+      <c r="F1778" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1778" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1778">
+        <v>4</v>
+      </c>
+      <c r="I1778">
+        <v>0.18181818199999999</v>
+      </c>
+      <c r="J1778">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1779" spans="1:10">
+      <c r="A1779" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1779" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1779" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1779" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1779">
+        <v>2021</v>
+      </c>
+      <c r="F1779" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1779" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1779">
+        <v>4</v>
+      </c>
+      <c r="I1779">
+        <v>0.18181818199999999</v>
+      </c>
+      <c r="J1779">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1780" spans="1:10">
+      <c r="A1780" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1780" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1780" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1780" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1780">
+        <v>2021</v>
+      </c>
+      <c r="F1780" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1780" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1780">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1781" spans="1:10">
+      <c r="A1781" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1781" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1781" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1781" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1781">
+        <v>2021</v>
+      </c>
+      <c r="F1781" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1781" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1781">
+        <v>3</v>
+      </c>
+      <c r="I1781">
+        <v>0.12121212100000001</v>
+      </c>
+      <c r="J1781">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1782" spans="1:10">
+      <c r="A1782" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1782" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1782" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1782" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1782">
+        <v>2021</v>
+      </c>
+      <c r="F1782" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1782" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1782">
+        <v>2</v>
+      </c>
+      <c r="I1782">
+        <v>9.0909090999999997E-2</v>
+      </c>
+      <c r="J1782">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1783" spans="1:10">
+      <c r="A1783" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1783" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1783" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1783" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1783">
+        <v>2021</v>
+      </c>
+      <c r="F1783" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1783" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1783">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1784" spans="1:10">
+      <c r="A1784" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1784" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1784" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1784" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1784">
+        <v>2021</v>
+      </c>
+      <c r="F1784" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1784" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1784">
+        <v>1</v>
+      </c>
+      <c r="I1784">
+        <v>3.0303030000000002E-2</v>
+      </c>
+      <c r="J1784">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>